<commit_message>
Added columns to the 2 tables
</commit_message>
<xml_diff>
--- a/Data Files/Data Center Analysis.xlsx
+++ b/Data Files/Data Center Analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\gsa\open.gsa.gov\Digital-Innovation-Hackathon-Fall2015\Files\DataCenter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\DataCenterMashup\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
   <si>
     <t>Parent Agency</t>
   </si>
@@ -384,6 +384,24 @@
       </rPr>
       <t>: Fields marked in yellow are common elements in the 2 objects so they will not be collected for data center information.</t>
     </r>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Created_By</t>
+  </si>
+  <si>
+    <t>Created_Dt</t>
+  </si>
+  <si>
+    <t>Updated_By</t>
+  </si>
+  <si>
+    <t>Updated_Dt</t>
   </si>
 </sst>
 </file>
@@ -445,7 +463,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -468,13 +486,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -486,6 +514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,22 +795,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="9" customWidth="1"/>
     <col min="3" max="3" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>96</v>
       </c>
       <c r="C1" t="s">
@@ -789,703 +818,736 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="2" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="2" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="8"/>
+      <c r="C28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="8"/>
+      <c r="C30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="4" t="s">
+      <c r="B31" s="8"/>
+      <c r="C31" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="4" t="s">
+      <c r="B32" s="8"/>
+      <c r="C32" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="4" t="s">
+      <c r="B33" s="8"/>
+      <c r="C33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="8"/>
+      <c r="C34" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="8"/>
+      <c r="C35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="4" t="s">
+      <c r="B36" s="8"/>
+      <c r="C36" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="4" t="s">
+      <c r="B37" s="8"/>
+      <c r="C37" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="4" t="s">
+      <c r="B38" s="8"/>
+      <c r="C38" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="4" t="s">
+      <c r="B39" s="8"/>
+      <c r="C39" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="4" t="s">
+      <c r="B40" s="8"/>
+      <c r="C40" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="4" t="s">
+      <c r="B41" s="8"/>
+      <c r="C41" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="4" t="s">
+      <c r="B42" s="8"/>
+      <c r="C42" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="4" t="s">
+      <c r="B43" s="8"/>
+      <c r="C43" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="4" t="s">
+      <c r="B44" s="8"/>
+      <c r="C44" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="4" t="s">
+      <c r="B45" s="8"/>
+      <c r="C45" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="4" t="s">
+      <c r="B46" s="8"/>
+      <c r="C46" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="4" t="s">
+      <c r="B47" s="8"/>
+      <c r="C47" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="4" t="s">
+      <c r="B48" s="8"/>
+      <c r="C48" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="4" t="s">
+      <c r="B49" s="8"/>
+      <c r="C49" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E49" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="4" t="s">
+      <c r="B50" s="8"/>
+      <c r="C50" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="E50" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="4" t="s">
+      <c r="B51" s="8"/>
+      <c r="C51" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E51" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="4" t="s">
+      <c r="B52" s="8"/>
+      <c r="C52" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E52" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="4" t="s">
+      <c r="B53" s="8"/>
+      <c r="C53" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="4" t="s">
+      <c r="B54" s="8"/>
+      <c r="C54" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="E54" s="12" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="4" t="s">
+      <c r="B55" s="8"/>
+      <c r="C55" s="3" t="s">
         <v>77</v>
       </c>
+      <c r="E55" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="4" t="s">
+      <c r="B56" s="8"/>
+      <c r="C56" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="E56" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="4" t="s">
+      <c r="B57" s="8"/>
+      <c r="C57" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="E57" s="12" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="4" t="s">
+      <c r="B58" s="8"/>
+      <c r="C58" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="E58" s="12" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="4" t="s">
+      <c r="B59" s="8"/>
+      <c r="C59" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="E59" s="12" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="4" t="s">
+      <c r="B60" s="8"/>
+      <c r="C60" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="4" t="s">
+      <c r="B61" s="8"/>
+      <c r="C61" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="4" t="s">
+      <c r="B62" s="8"/>
+      <c r="C62" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="11" t="s">
+      <c r="B63" s="8"/>
+      <c r="C63" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C64" s="2" t="s">
+      <c r="A64" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="9"/>
-      <c r="C65" s="4" t="s">
+      <c r="A65" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="3" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>